<commit_message>
Updated with the interactive charts and new CSS
</commit_message>
<xml_diff>
--- a/datasets/cleandata.xlsx
+++ b/datasets/cleandata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonya/Documents/NM2207/web/finalProject/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC087D7-7991-A84D-BA2C-C96FA20B9E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459917C9-1F30-FF41-8A22-78A74B3144FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1760" yWindow="1240" windowWidth="27640" windowHeight="16000" xr2:uid="{B0305598-C37C-4442-8B54-72AAA8529E06}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
   <si>
     <t>2000</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>1990</t>
+  </si>
+  <si>
+    <t>Average no.</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -465,13 +468,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -494,13 +517,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -819,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01793D13-6614-5B40-9D56-AE8896967020}">
-  <dimension ref="A1:AH22"/>
+  <dimension ref="A1:AJ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="AJ4" sqref="AJ4:AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -830,7 +859,7 @@
     <col min="1" max="1" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -933,8 +962,11 @@
       <c r="AH1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI1" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>23</v>
       </c>
@@ -1037,8 +1069,12 @@
       <c r="AH2" s="2">
         <v>5637022</v>
       </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI2" s="23">
+        <f>AVERAGE(B2:AH2)</f>
+        <v>4546774.8787878789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>24</v>
       </c>
@@ -1141,8 +1177,12 @@
       <c r="AH3" s="2">
         <v>4073239</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI3" s="23">
+        <f>AVERAGE(B3:AH3)</f>
+        <v>3502913.8787878789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>25</v>
       </c>
@@ -1245,8 +1285,15 @@
       <c r="AH4" s="2">
         <v>3553749</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI4" s="23">
+        <f t="shared" ref="AI3:AI6" si="0">AVERAGE(B4:AH4)</f>
+        <v>3121499.8787878789</v>
+      </c>
+      <c r="AJ4" s="24">
+        <v>3121500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>26</v>
       </c>
@@ -1349,8 +1396,15 @@
       <c r="AH5" s="2">
         <v>519490</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI5" s="23">
+        <f t="shared" si="0"/>
+        <v>381413.90909090912</v>
+      </c>
+      <c r="AJ5" s="24">
+        <v>381414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>27</v>
       </c>
@@ -1453,8 +1507,15 @@
       <c r="AH6" s="2">
         <v>1563783</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="AI6" s="23">
+        <f t="shared" si="0"/>
+        <v>1043861</v>
+      </c>
+      <c r="AJ6" s="24">
+        <v>1043861</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -1479,110 +1540,34 @@
       <c r="V9" s="19"/>
       <c r="W9" s="19"/>
       <c r="X9" s="19"/>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="20"/>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="22"/>
-      <c r="X10" s="22"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
-      <c r="AA10" s="20"/>
-      <c r="AB10" s="20"/>
-      <c r="AC10" s="20"/>
-      <c r="AD10" s="20"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="20"/>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
-      <c r="AC11" s="20"/>
-      <c r="AD11" s="20"/>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="20"/>
-      <c r="U12" s="20"/>
-      <c r="V12" s="20"/>
-      <c r="W12" s="20"/>
-      <c r="X12" s="20"/>
-      <c r="Y12" s="20"/>
-      <c r="Z12" s="20"/>
-      <c r="AA12" s="20"/>
-      <c r="AB12" s="20"/>
-      <c r="AC12" s="20"/>
-      <c r="AD12" s="20"/>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -1607,110 +1592,34 @@
       <c r="V13" s="19"/>
       <c r="W13" s="19"/>
       <c r="X13" s="19"/>
-      <c r="Y13" s="20"/>
-      <c r="Z13" s="20"/>
-      <c r="AA13" s="20"/>
-      <c r="AB13" s="20"/>
-      <c r="AC13" s="20"/>
-      <c r="AD13" s="20"/>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="22"/>
-      <c r="U14" s="22"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="22"/>
-      <c r="X14" s="22"/>
-      <c r="Y14" s="20"/>
-      <c r="Z14" s="20"/>
-      <c r="AA14" s="20"/>
-      <c r="AB14" s="20"/>
-      <c r="AC14" s="20"/>
-      <c r="AD14" s="20"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="20"/>
-      <c r="V15" s="20"/>
-      <c r="W15" s="20"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="20"/>
-      <c r="Z15" s="20"/>
-      <c r="AA15" s="20"/>
-      <c r="AB15" s="20"/>
-      <c r="AC15" s="20"/>
-      <c r="AD15" s="20"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="20"/>
-      <c r="U16" s="20"/>
-      <c r="V16" s="20"/>
-      <c r="W16" s="20"/>
-      <c r="X16" s="20"/>
-      <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
-      <c r="AA16" s="20"/>
-      <c r="AB16" s="20"/>
-      <c r="AC16" s="20"/>
-      <c r="AD16" s="20"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="21"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -1735,172 +1644,32 @@
       <c r="V17" s="19"/>
       <c r="W17" s="19"/>
       <c r="X17" s="19"/>
-      <c r="Y17" s="20"/>
-      <c r="Z17" s="20"/>
-      <c r="AA17" s="20"/>
-      <c r="AB17" s="20"/>
-      <c r="AC17" s="20"/>
-      <c r="AD17" s="20"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-      <c r="T18" s="22"/>
-      <c r="U18" s="22"/>
-      <c r="V18" s="22"/>
-      <c r="W18" s="22"/>
-      <c r="X18" s="22"/>
-      <c r="Y18" s="20"/>
-      <c r="Z18" s="20"/>
-      <c r="AA18" s="20"/>
-      <c r="AB18" s="20"/>
-      <c r="AC18" s="20"/>
-      <c r="AD18" s="20"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="20"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="20"/>
-      <c r="X19" s="20"/>
-      <c r="Y19" s="20"/>
-      <c r="Z19" s="20"/>
-      <c r="AA19" s="20"/>
-      <c r="AB19" s="20"/>
-      <c r="AC19" s="20"/>
-      <c r="AD19" s="20"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="20"/>
-      <c r="Z20" s="20"/>
-      <c r="AA20" s="20"/>
-      <c r="AB20" s="20"/>
-      <c r="AC20" s="20"/>
-      <c r="AD20" s="20"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="20"/>
-      <c r="U21" s="20"/>
-      <c r="V21" s="20"/>
-      <c r="W21" s="20"/>
-      <c r="X21" s="20"/>
-      <c r="Y21" s="20"/>
-      <c r="Z21" s="20"/>
-      <c r="AA21" s="20"/>
-      <c r="AB21" s="20"/>
-      <c r="AC21" s="20"/>
-      <c r="AD21" s="20"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="W22" s="20"/>
-      <c r="X22" s="20"/>
-      <c r="Y22" s="20"/>
-      <c r="Z22" s="20"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="20"/>
-      <c r="AD22" s="20"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="B27:AR32">

</xml_diff>